<commit_message>
fully brought back multis
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/Brackets.xlsx
+++ b/thesis-tex/excels/Brackets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8538CECA-011E-436E-B5E8-CF6B4B0AA51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD38CF4-DE25-4839-8523-5CFDB08FB86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="19" activeTab="20" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
@@ -102,7 +102,6 @@
     <definedName name="solver_ver" localSheetId="25" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2146,8 +2145,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2156,21 +2165,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2191,13 +2200,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2206,16 +2209,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9635,16 +9634,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="102"/>
+      <c r="E5" s="103"/>
       <c r="F5" s="29"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="101" t="s">
+      <c r="H5" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="102"/>
+      <c r="I5" s="103"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -11642,7 +11641,7 @@
   <dimension ref="C3:AU41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="V3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11771,7 +11770,7 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="117" t="s">
+      <c r="AC5" s="94" t="s">
         <v>40</v>
       </c>
       <c r="AD5" s="1"/>
@@ -11780,7 +11779,7 @@
         <v>1</v>
       </c>
       <c r="AG5" s="1"/>
-      <c r="AH5" s="117" t="s">
+      <c r="AH5" s="94" t="s">
         <v>41</v>
       </c>
       <c r="AI5" s="1"/>
@@ -11789,7 +11788,7 @@
         <v>1</v>
       </c>
       <c r="AL5" s="1"/>
-      <c r="AM5" s="117" t="s">
+      <c r="AM5" s="94" t="s">
         <v>42</v>
       </c>
       <c r="AN5" s="1"/>
@@ -11798,7 +11797,7 @@
         <v>1</v>
       </c>
       <c r="AQ5" s="1"/>
-      <c r="AR5" s="117" t="s">
+      <c r="AR5" s="94" t="s">
         <v>43</v>
       </c>
       <c r="AS5" s="1"/>
@@ -12563,7 +12562,7 @@
         <v>1</v>
       </c>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="117" t="s">
+      <c r="AC21" s="94" t="s">
         <v>185</v>
       </c>
       <c r="AD21" s="1"/>
@@ -12572,7 +12571,7 @@
         <v>1</v>
       </c>
       <c r="AG21" s="1"/>
-      <c r="AH21" s="117" t="s">
+      <c r="AH21" s="94" t="s">
         <v>186</v>
       </c>
       <c r="AI21" s="1"/>
@@ -12581,7 +12580,7 @@
         <v>1</v>
       </c>
       <c r="AL21" s="1"/>
-      <c r="AM21" s="117" t="s">
+      <c r="AM21" s="94" t="s">
         <v>187</v>
       </c>
       <c r="AN21" s="1"/>
@@ -12590,7 +12589,7 @@
         <v>1</v>
       </c>
       <c r="AQ21" s="1"/>
-      <c r="AR21" s="117" t="s">
+      <c r="AR21" s="94" t="s">
         <v>188</v>
       </c>
       <c r="AS21" s="1"/>
@@ -13599,25 +13598,25 @@
     </row>
     <row r="2" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="109" t="s">
+      <c r="D2" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="111"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="106"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="109" t="s">
+      <c r="M2" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="111"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="106"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
@@ -13626,11 +13625,11 @@
       <c r="D3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="103" t="s">
+      <c r="E3" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="109"/>
       <c r="H3" s="44" t="s">
         <v>112</v>
       </c>
@@ -13643,11 +13642,11 @@
       <c r="M3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="N3" s="103" t="s">
+      <c r="N3" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="104"/>
-      <c r="P3" s="105"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="109"/>
       <c r="Q3" s="44" t="s">
         <v>112</v>
       </c>
@@ -13662,11 +13661,11 @@
       <c r="D4" s="54">
         <v>1</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="109"/>
       <c r="H4" s="44">
         <v>2</v>
       </c>
@@ -13680,11 +13679,11 @@
       <c r="M4" s="54">
         <v>1</v>
       </c>
-      <c r="N4" s="103" t="s">
+      <c r="N4" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="O4" s="104"/>
-      <c r="P4" s="105"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="109"/>
       <c r="Q4" s="44">
         <v>4</v>
       </c>
@@ -13700,11 +13699,11 @@
       <c r="D5" s="54">
         <v>2</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="105"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="109"/>
       <c r="H5" s="44">
         <v>2</v>
       </c>
@@ -13718,11 +13717,11 @@
       <c r="M5" s="54">
         <v>2</v>
       </c>
-      <c r="N5" s="103" t="s">
+      <c r="N5" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="104"/>
-      <c r="P5" s="105"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="109"/>
       <c r="Q5" s="44">
         <v>3</v>
       </c>
@@ -13738,11 +13737,11 @@
       <c r="D6" s="54">
         <v>3</v>
       </c>
-      <c r="E6" s="103" t="s">
+      <c r="E6" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="109"/>
       <c r="H6" s="44">
         <v>2</v>
       </c>
@@ -13756,11 +13755,11 @@
       <c r="M6" s="54">
         <v>3</v>
       </c>
-      <c r="N6" s="103" t="s">
+      <c r="N6" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="104"/>
-      <c r="P6" s="105"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="109"/>
       <c r="Q6" s="44">
         <v>2</v>
       </c>
@@ -13776,11 +13775,11 @@
       <c r="D7" s="54">
         <v>4</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="E7" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="105"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="109"/>
       <c r="H7" s="44">
         <v>2</v>
       </c>
@@ -13794,11 +13793,11 @@
       <c r="M7" s="54">
         <v>4</v>
       </c>
-      <c r="N7" s="103" t="s">
+      <c r="N7" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="O7" s="104"/>
-      <c r="P7" s="105"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="109"/>
       <c r="Q7" s="44">
         <v>1</v>
       </c>
@@ -13814,11 +13813,11 @@
       <c r="D8" s="56">
         <v>5</v>
       </c>
-      <c r="E8" s="106" t="s">
+      <c r="E8" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="107"/>
-      <c r="G8" s="108"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
       <c r="H8" s="57">
         <v>2</v>
       </c>
@@ -13832,11 +13831,11 @@
       <c r="M8" s="56">
         <v>5</v>
       </c>
-      <c r="N8" s="106" t="s">
+      <c r="N8" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="107"/>
-      <c r="P8" s="108"/>
+      <c r="O8" s="111"/>
+      <c r="P8" s="112"/>
       <c r="Q8" s="57">
         <v>0</v>
       </c>
@@ -13869,25 +13868,25 @@
     </row>
     <row r="10" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="109" t="s">
+      <c r="D10" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="111"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="106"/>
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="109" t="s">
+      <c r="M10" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="N10" s="110"/>
-      <c r="O10" s="110"/>
-      <c r="P10" s="110"/>
-      <c r="Q10" s="110"/>
-      <c r="R10" s="111"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="105"/>
+      <c r="Q10" s="105"/>
+      <c r="R10" s="106"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
@@ -13896,11 +13895,11 @@
       <c r="D11" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="103" t="s">
+      <c r="E11" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="104"/>
-      <c r="G11" s="105"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="109"/>
       <c r="H11" s="44" t="s">
         <v>112</v>
       </c>
@@ -13913,11 +13912,11 @@
       <c r="M11" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="103" t="s">
+      <c r="N11" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="104"/>
-      <c r="P11" s="105"/>
+      <c r="O11" s="108"/>
+      <c r="P11" s="109"/>
       <c r="Q11" s="44" t="s">
         <v>112</v>
       </c>
@@ -13932,11 +13931,11 @@
       <c r="D12" s="54">
         <v>1</v>
       </c>
-      <c r="E12" s="103" t="s">
+      <c r="E12" s="107" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="104"/>
-      <c r="G12" s="105"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="109"/>
       <c r="H12" s="44">
         <v>3</v>
       </c>
@@ -13950,11 +13949,11 @@
       <c r="M12" s="54">
         <v>1</v>
       </c>
-      <c r="N12" s="103" t="s">
+      <c r="N12" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="O12" s="104"/>
-      <c r="P12" s="105"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="109"/>
       <c r="Q12" s="44">
         <v>4</v>
       </c>
@@ -13970,11 +13969,11 @@
       <c r="D13" s="54">
         <v>2</v>
       </c>
-      <c r="E13" s="103" t="s">
+      <c r="E13" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="109"/>
       <c r="H13" s="44">
         <v>3</v>
       </c>
@@ -13988,11 +13987,11 @@
       <c r="M13" s="54">
         <v>2</v>
       </c>
-      <c r="N13" s="103" t="s">
+      <c r="N13" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="O13" s="104"/>
-      <c r="P13" s="105"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="109"/>
       <c r="Q13" s="44">
         <v>3</v>
       </c>
@@ -14008,11 +14007,11 @@
       <c r="D14" s="54">
         <v>3</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="104"/>
-      <c r="G14" s="105"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="109"/>
       <c r="H14" s="44">
         <v>2</v>
       </c>
@@ -14026,11 +14025,11 @@
       <c r="M14" s="54">
         <v>3</v>
       </c>
-      <c r="N14" s="103" t="s">
+      <c r="N14" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="O14" s="104"/>
-      <c r="P14" s="105"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="109"/>
       <c r="Q14" s="44">
         <v>2</v>
       </c>
@@ -14046,11 +14045,11 @@
       <c r="D15" s="54">
         <v>4</v>
       </c>
-      <c r="E15" s="103" t="s">
+      <c r="E15" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="F15" s="104"/>
-      <c r="G15" s="105"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="109"/>
       <c r="H15" s="44">
         <v>1</v>
       </c>
@@ -14064,11 +14063,11 @@
       <c r="M15" s="54">
         <v>4</v>
       </c>
-      <c r="N15" s="103" t="s">
+      <c r="N15" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="O15" s="104"/>
-      <c r="P15" s="105"/>
+      <c r="O15" s="108"/>
+      <c r="P15" s="109"/>
       <c r="Q15" s="44">
         <v>1</v>
       </c>
@@ -14084,11 +14083,11 @@
       <c r="D16" s="56">
         <v>5</v>
       </c>
-      <c r="E16" s="106" t="s">
+      <c r="E16" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="107"/>
-      <c r="G16" s="108"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="112"/>
       <c r="H16" s="57">
         <v>1</v>
       </c>
@@ -14102,11 +14101,11 @@
       <c r="M16" s="56">
         <v>5</v>
       </c>
-      <c r="N16" s="106" t="s">
+      <c r="N16" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="O16" s="107"/>
-      <c r="P16" s="108"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="112"/>
       <c r="Q16" s="57">
         <v>0</v>
       </c>
@@ -15819,6 +15818,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="M2:R2"/>
     <mergeCell ref="D10:I10"/>
@@ -15835,18 +15846,6 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16471,26 +16470,26 @@
     </row>
     <row r="2" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="109" t="s">
+      <c r="D2" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="111"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="106"/>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="109" t="s">
+      <c r="N2" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="111"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="106"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
@@ -16499,29 +16498,29 @@
       <c r="D3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="103" t="s">
+      <c r="E3" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="104"/>
-      <c r="G3" s="105"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="109"/>
       <c r="H3" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="112"/>
+      <c r="J3" s="114"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
       <c r="M3" s="1"/>
       <c r="N3" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="O3" s="103" t="s">
+      <c r="O3" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="105"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="109"/>
       <c r="R3" s="44" t="s">
         <v>112</v>
       </c>
@@ -16536,29 +16535,29 @@
       <c r="D4" s="54">
         <v>1</v>
       </c>
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="109"/>
       <c r="H4" s="44">
         <v>5</v>
       </c>
-      <c r="I4" s="103">
-        <v>0</v>
-      </c>
-      <c r="J4" s="112"/>
+      <c r="I4" s="107">
+        <v>0</v>
+      </c>
+      <c r="J4" s="114"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="1"/>
       <c r="N4" s="54">
         <v>1</v>
       </c>
-      <c r="O4" s="103" t="s">
+      <c r="O4" s="107" t="s">
         <v>140</v>
       </c>
-      <c r="P4" s="104"/>
-      <c r="Q4" s="105"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="109"/>
       <c r="R4" s="44">
         <v>5</v>
       </c>
@@ -16573,29 +16572,29 @@
       <c r="D5" s="54">
         <v>2</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="105"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="109"/>
       <c r="H5" s="44">
         <v>4</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5" s="107">
         <v>1</v>
       </c>
-      <c r="J5" s="112"/>
+      <c r="J5" s="114"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="1"/>
       <c r="N5" s="54">
         <v>2</v>
       </c>
-      <c r="O5" s="103" t="s">
+      <c r="O5" s="107" t="s">
         <v>141</v>
       </c>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="105"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="109"/>
       <c r="R5" s="44">
         <v>3</v>
       </c>
@@ -16610,29 +16609,29 @@
       <c r="D6" s="54">
         <v>3</v>
       </c>
-      <c r="E6" s="103" t="s">
+      <c r="E6" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="109"/>
       <c r="H6" s="44">
         <v>3</v>
       </c>
-      <c r="I6" s="103">
+      <c r="I6" s="107">
         <v>2</v>
       </c>
-      <c r="J6" s="112"/>
+      <c r="J6" s="114"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
       <c r="M6" s="1"/>
       <c r="N6" s="54">
         <v>3</v>
       </c>
-      <c r="O6" s="103" t="s">
+      <c r="O6" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="105"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="109"/>
       <c r="R6" s="44">
         <v>3</v>
       </c>
@@ -16647,29 +16646,29 @@
       <c r="D7" s="54">
         <v>4</v>
       </c>
-      <c r="E7" s="103" t="s">
+      <c r="E7" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="104"/>
-      <c r="G7" s="105"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="109"/>
       <c r="H7" s="44">
         <v>2</v>
       </c>
-      <c r="I7" s="103">
+      <c r="I7" s="107">
         <v>3</v>
       </c>
-      <c r="J7" s="112"/>
+      <c r="J7" s="114"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="1"/>
       <c r="N7" s="54">
         <v>4</v>
       </c>
-      <c r="O7" s="103" t="s">
+      <c r="O7" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="P7" s="104"/>
-      <c r="Q7" s="105"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="109"/>
       <c r="R7" s="44">
         <v>3</v>
       </c>
@@ -16684,29 +16683,29 @@
       <c r="D8" s="61">
         <v>5</v>
       </c>
-      <c r="E8" s="103" t="s">
+      <c r="E8" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="104"/>
-      <c r="G8" s="105"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="109"/>
       <c r="H8" s="59">
         <v>1</v>
       </c>
-      <c r="I8" s="103">
+      <c r="I8" s="107">
         <v>4</v>
       </c>
-      <c r="J8" s="112"/>
+      <c r="J8" s="114"/>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
       <c r="M8" s="1"/>
       <c r="N8" s="61">
         <v>5</v>
       </c>
-      <c r="O8" s="103" t="s">
+      <c r="O8" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="105"/>
+      <c r="P8" s="108"/>
+      <c r="Q8" s="109"/>
       <c r="R8" s="59">
         <v>1</v>
       </c>
@@ -16721,29 +16720,29 @@
       <c r="D9" s="56">
         <v>6</v>
       </c>
-      <c r="E9" s="106" t="s">
+      <c r="E9" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="107"/>
-      <c r="G9" s="108"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="112"/>
       <c r="H9" s="57">
         <v>0</v>
       </c>
-      <c r="I9" s="106">
+      <c r="I9" s="110">
         <v>5</v>
       </c>
-      <c r="J9" s="113"/>
+      <c r="J9" s="115"/>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="1"/>
       <c r="N9" s="56">
         <v>6</v>
       </c>
-      <c r="O9" s="106" t="s">
+      <c r="O9" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="P9" s="107"/>
-      <c r="Q9" s="108"/>
+      <c r="P9" s="111"/>
+      <c r="Q9" s="112"/>
       <c r="R9" s="57">
         <v>0</v>
       </c>
@@ -18538,14 +18537,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="O9:Q9"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="E6:G6"/>
@@ -18555,12 +18552,14 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19323,12 +19322,12 @@
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="T13" s="115" t="s">
+      <c r="T13" s="116" t="s">
         <v>164</v>
       </c>
-      <c r="U13" s="115"/>
-      <c r="V13" s="115"/>
-      <c r="W13" s="115"/>
+      <c r="U13" s="116"/>
+      <c r="V13" s="116"/>
+      <c r="W13" s="116"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -35739,10 +35738,10 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="116" t="s">
+      <c r="F33" s="117" t="s">
         <v>240</v>
       </c>
-      <c r="G33" s="116"/>
+      <c r="G33" s="117"/>
       <c r="H33" s="1"/>
       <c r="I33" s="70"/>
       <c r="J33" s="1" t="s">
@@ -35751,10 +35750,10 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="116" t="s">
+      <c r="N33" s="117" t="s">
         <v>240</v>
       </c>
-      <c r="O33" s="116"/>
+      <c r="O33" s="117"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
@@ -35764,16 +35763,16 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
       <c r="H34" s="1"/>
       <c r="I34" s="70"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="116"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="117"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
@@ -36180,8 +36179,8 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="116"/>
-      <c r="G53" s="116"/>
+      <c r="F53" s="117"/>
+      <c r="G53" s="117"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1" t="s">
@@ -36190,24 +36189,24 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="116"/>
-      <c r="O53" s="116"/>
+      <c r="N53" s="117"/>
+      <c r="O53" s="117"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="116"/>
-      <c r="G54" s="116"/>
+      <c r="F54" s="117"/>
+      <c r="G54" s="117"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="116"/>
-      <c r="O54" s="116"/>
+      <c r="N54" s="117"/>
+      <c r="O54" s="117"/>
     </row>
     <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I55" s="1"/>
@@ -56944,7 +56943,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ6 BZ4 BZ8 BZ10 BZ12 BZ14 BZ16 BZ18 BZ20 BZ22 BZ24 BZ26 BZ28 BZ30 BZ32 BZ34 BZ36 BZ38 BZ40 BZ42 BZ44 BZ46 BZ48 BZ50 BZ52 BZ54 BZ56 BZ58 BZ60 BZ62 BZ64 BZ66 BZ68 BZ70 BZ72 BZ74 BZ76 BZ78 BZ80 BZ82 BZ84 BZ86 BZ88 BZ90 BZ92 BZ94 BZ96 BZ98 BZ100 BZ102 BZ104">
+  <conditionalFormatting sqref="BZ4 BZ6 BZ8 BZ10 BZ12 BZ14 BZ16 BZ18 BZ20 BZ22 BZ24 BZ26 BZ28 BZ30 BZ32 BZ34 BZ36 BZ38 BZ40 BZ42 BZ44 BZ46 BZ48 BZ50 BZ52 BZ54 BZ56 BZ58 BZ60 BZ62 BZ64 BZ66 BZ68 BZ70 BZ72 BZ74 BZ76 BZ78 BZ80 BZ82 BZ84 BZ86 BZ88 BZ90 BZ92 BZ94 BZ96 BZ98 BZ100 BZ102 BZ104">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -56956,7 +56955,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA6 CA4 CA8 CA10 CA12 CA14 CA16 CA18 CA20 CA22 CA24 CA26 CA28 CA30 CA32 CA34 CA36 CA38 CA40 CA42 CA44 CA46 CA48 CA50 CA52 CA54 CA56 CA58 CA60 CA62 CA64 CA66 CA68 CA70 CA72 CA74 CA76 CA78 CA80 CA82 CA84 CA86 CA88 CA90 CA92 CA94 CA96 CA98 CA100 CA102 CA104">
+  <conditionalFormatting sqref="CA4 CA6 CA8 CA10 CA12 CA14 CA16 CA18 CA20 CA22 CA24 CA26 CA28 CA30 CA32 CA34 CA36 CA38 CA40 CA42 CA44 CA46 CA48 CA50 CA52 CA54 CA56 CA58 CA60 CA62 CA64 CA66 CA68 CA70 CA72 CA74 CA76 CA78 CA80 CA82 CA84 CA86 CA88 CA90 CA92 CA94 CA96 CA98 CA100 CA102 CA104">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -56968,7 +56967,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CB6 CB4 CB8 CB10 CB12 CB14 CB16 CB18 CB20 CB22 CB24 CB26 CB28 CB30 CB32 CB34 CB36 CB38 CB40 CB42 CB44 CB46 CB48 CB50 CB52 CB54 CB56 CB58 CB60 CB62 CB64 CB66 CB68 CB70 CB72 CB74 CB76 CB78 CB80 CB82 CB84 CB86 CB88 CB90 CB92 CB94 CB96 CB98 CB100 CB102 CB104">
+  <conditionalFormatting sqref="CB4 CB6 CB8 CB10 CB12 CB14 CB16 CB18 CB20 CB22 CB24 CB26 CB28 CB30 CB32 CB34 CB36 CB38 CB40 CB42 CB44 CB46 CB48 CB50 CB52 CB54 CB56 CB58 CB60 CB62 CB64 CB66 CB68 CB70 CB72 CB74 CB76 CB78 CB80 CB82 CB84 CB86 CB88 CB90 CB92 CB94 CB96 CB98 CB100 CB102 CB104">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -56980,7 +56979,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CC6 CC4 CC8 CC10 CC12 CC14 CC16 CC18 CC20 CC22 CC24 CC26 CC28 CC30 CC32 CC34 CC36 CC38 CC40 CC42 CC44 CC46 CC48 CC50 CC52 CC54 CC56 CC58 CC60 CC62 CC64 CC66 CC68 CC70 CC72 CC74 CC76 CC78 CC80 CC82 CC84 CC86 CC88 CC90 CC92 CC94 CC96 CC98 CC100 CC102 CC104">
+  <conditionalFormatting sqref="CC4 CC6 CC8 CC10 CC12 CC14 CC16 CC18 CC20 CC22 CC24 CC26 CC28 CC30 CC32 CC34 CC36 CC38 CC40 CC42 CC44 CC46 CC48 CC50 CC52 CC54 CC56 CC58 CC60 CC62 CC64 CC66 CC68 CC70 CC72 CC74 CC76 CC78 CC80 CC82 CC84 CC86 CC88 CC90 CC92 CC94 CC96 CC98 CC100 CC102 CC104">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -56992,7 +56991,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD6 CD4 CD8 CD10 CD12 CD14 CD16 CD18 CD20 CD22 CD24 CD26 CD28 CD30 CD32 CD34 CD36 CD38 CD40 CD42 CD44 CD46 CD48 CD50 CD52 CD54 CD56 CD58 CD60 CD62 CD64 CD66 CD68 CD70 CD72 CD74 CD76 CD78 CD80 CD82 CD84 CD86 CD88 CD90 CD92 CD94 CD96 CD98 CD100 CD102 CD104">
+  <conditionalFormatting sqref="CD4 CD6 CD8 CD10 CD12 CD14 CD16 CD18 CD20 CD22 CD24 CD26 CD28 CD30 CD32 CD34 CD36 CD38 CD40 CD42 CD44 CD46 CD48 CD50 CD52 CD54 CD56 CD58 CD60 CD62 CD64 CD66 CD68 CD70 CD72 CD74 CD76 CD78 CD80 CD82 CD84 CD86 CD88 CD90 CD92 CD94 CD96 CD98 CD100 CD102 CD104">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -57004,7 +57003,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CE6 CE4 CE8 CE10 CE12 CE14 CE16 CE18 CE20 CE22 CE24 CE26 CE28 CE30 CE32 CE34 CE36 CE38 CE40 CE42 CE44 CE46 CE48 CE50 CE52 CE54 CE56 CE58 CE60 CE62 CE64 CE66 CE68 CE70 CE72 CE74 CE76 CE78 CE80 CE82 CE84 CE86 CE88 CE90 CE92 CE94 CE96 CE98 CE100 CE102 CE104">
+  <conditionalFormatting sqref="CE4 CE6 CE8 CE10 CE12 CE14 CE16 CE18 CE20 CE22 CE24 CE26 CE28 CE30 CE32 CE34 CE36 CE38 CE40 CE42 CE44 CE46 CE48 CE50 CE52 CE54 CE56 CE58 CE60 CE62 CE64 CE66 CE68 CE70 CE72 CE74 CE76 CE78 CE80 CE82 CE84 CE86 CE88 CE90 CE92 CE94 CE96 CE98 CE100 CE102 CE104">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -60304,7 +60303,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="94"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -60312,7 +60311,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="94"/>
+      <c r="D9" s="95"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -60346,7 +60345,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="94"/>
+      <c r="D12" s="95"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -60354,7 +60353,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="94"/>
+      <c r="D13" s="95"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -60388,7 +60387,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="94"/>
+      <c r="D16" s="95"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -60396,7 +60395,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="94"/>
+      <c r="D17" s="95"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -60492,7 +60491,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="94"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -60502,7 +60501,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="94"/>
+      <c r="D9" s="95"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -60517,8 +60516,8 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="100"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="96"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
@@ -60527,8 +60526,8 @@
       <c r="B11" s="97"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="100"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="96"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
@@ -60537,7 +60536,7 @@
       <c r="B12" s="98"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="100"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -60549,33 +60548,33 @@
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="100"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="95" t="s">
+      <c r="I13" s="99" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="97"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="99"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="101"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="95"/>
+      <c r="I14" s="99"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
       <c r="C15" s="98"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="99"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="101"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="96"/>
+      <c r="I15" s="100"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -60584,7 +60583,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="94"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -60594,7 +60593,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="94"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -60632,9 +60631,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -60642,9 +60641,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
@@ -60663,17 +60662,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove spaces from filenames
</commit_message>
<xml_diff>
--- a/thesis-tex/excels/Brackets.xlsx
+++ b/thesis-tex/excels/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EADBA8A-C942-4918-86CA-02B71F6918DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126578A-E968-4469-92EA-BD81FD34B51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="32" activeTab="38" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="cfp" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,6 @@
     <definedName name="solver_ver" localSheetId="24" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5199,7 +5198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -5445,19 +5444,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5478,13 +5473,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5494,45 +5498,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6521,7 +6489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68B215-176C-47A9-BC65-E5FAC0AEE706}">
   <dimension ref="B2:U19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -6909,7 +6877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
   <dimension ref="B4:BT40"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AJ1" sqref="AJ1:AN1048576"/>
     </sheetView>
   </sheetViews>
@@ -12456,10 +12424,6 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
       <c r="Q1" s="89"/>
       <c r="R1" s="89"/>
       <c r="S1" s="89"/>
@@ -12482,10 +12446,10 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -12515,10 +12479,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -12550,10 +12514,10 @@
       <c r="A4" s="83"/>
       <c r="B4" s="83"/>
       <c r="C4" s="23"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="83"/>
       <c r="I4" s="83"/>
       <c r="J4" s="83"/>
@@ -12587,10 +12551,10 @@
       <c r="C5" s="23" t="s">
         <v>447</v>
       </c>
-      <c r="D5" s="134"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="83"/>
       <c r="I5" s="83"/>
       <c r="J5" s="83"/>
@@ -12622,12 +12586,12 @@
       <c r="A6" s="89"/>
       <c r="B6" s="83"/>
       <c r="C6" s="91"/>
-      <c r="D6" s="134" t="s">
+      <c r="D6" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="83"/>
       <c r="I6" s="83"/>
       <c r="J6" s="83"/>
@@ -12661,10 +12625,10 @@
       <c r="C7" s="88" t="s">
         <v>448</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="83"/>
       <c r="I7" s="83"/>
       <c r="J7" s="83"/>
@@ -12706,12 +12670,12 @@
       <c r="A8" s="89"/>
       <c r="B8" s="83"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="138" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="83"/>
       <c r="I8" s="83"/>
       <c r="J8" s="83"/>
@@ -12745,17 +12709,17 @@
       <c r="C9" s="23" t="s">
         <v>449</v>
       </c>
-      <c r="D9" s="134"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
       <c r="O9" s="83"/>
       <c r="P9" s="83"/>
       <c r="Q9" s="23"/>
@@ -12782,19 +12746,19 @@
       <c r="A10" s="89"/>
       <c r="B10" s="83"/>
       <c r="C10" s="91"/>
-      <c r="D10" s="134" t="s">
+      <c r="D10" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="129"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="83"/>
       <c r="P10" s="83"/>
       <c r="Q10" s="23"/>
@@ -12821,17 +12785,17 @@
       <c r="C11" s="88" t="s">
         <v>450</v>
       </c>
-      <c r="D11" s="137"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="129"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
       <c r="O11" s="83"/>
       <c r="P11" s="83"/>
       <c r="Q11" s="23"/>
@@ -12866,19 +12830,19 @@
       <c r="A12" s="89"/>
       <c r="B12" s="83"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="138" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="140"/>
-      <c r="H12" s="129"/>
-      <c r="I12" s="129"/>
-      <c r="J12" s="129"/>
-      <c r="K12" s="129"/>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
-      <c r="N12" s="129"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
       <c r="O12" s="83"/>
       <c r="P12" s="83"/>
       <c r="Q12" s="23"/>
@@ -12905,17 +12869,17 @@
       <c r="C13" s="23" t="s">
         <v>453</v>
       </c>
-      <c r="D13" s="134"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="139"/>
-      <c r="G13" s="138"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="83"/>
+      <c r="N13" s="83"/>
       <c r="O13" s="83"/>
       <c r="P13" s="83"/>
       <c r="Q13" s="23"/>
@@ -12940,19 +12904,19 @@
       <c r="A14" s="89"/>
       <c r="B14" s="83"/>
       <c r="C14" s="91"/>
-      <c r="D14" s="134" t="s">
+      <c r="D14" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="E14" s="136"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="138"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="129"/>
-      <c r="K14" s="129"/>
-      <c r="L14" s="129"/>
-      <c r="M14" s="129"/>
-      <c r="N14" s="129"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="83"/>
       <c r="O14" s="83"/>
       <c r="P14" s="83"/>
       <c r="Q14" s="6"/>
@@ -12979,17 +12943,17 @@
       <c r="C15" s="88" t="s">
         <v>452</v>
       </c>
-      <c r="D15" s="137"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
-      <c r="K15" s="129"/>
-      <c r="L15" s="129"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
       <c r="O15" s="83"/>
       <c r="P15" s="83"/>
       <c r="Q15" s="6"/>
@@ -13014,19 +12978,19 @@
       <c r="A16" s="89"/>
       <c r="B16" s="83"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="138" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="129"/>
-      <c r="I16" s="129"/>
-      <c r="J16" s="129"/>
-      <c r="K16" s="129"/>
-      <c r="L16" s="129"/>
-      <c r="M16" s="129"/>
-      <c r="N16" s="129"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="83"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="83"/>
       <c r="O16" s="83"/>
       <c r="P16" s="83"/>
       <c r="Q16" s="6"/>
@@ -13053,11 +13017,11 @@
       <c r="C17" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="D17" s="134"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="129"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="83"/>
       <c r="I17" s="83"/>
       <c r="J17" s="83"/>
       <c r="K17" s="83"/>
@@ -13088,13 +13052,13 @@
       <c r="A18" s="89"/>
       <c r="B18" s="83"/>
       <c r="C18" s="91"/>
-      <c r="D18" s="134" t="s">
+      <c r="D18" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="138"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="129"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="83"/>
       <c r="J18" s="83"/>
       <c r="K18" s="83"/>
@@ -13110,11 +13074,11 @@
       <c r="C19" s="88" t="s">
         <v>454</v>
       </c>
-      <c r="D19" s="137"/>
-      <c r="E19" s="136"/>
-      <c r="F19" s="136"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="129"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="83"/>
       <c r="I19" s="83"/>
       <c r="J19" s="83"/>
       <c r="K19" s="83"/>
@@ -13128,13 +13092,13 @@
       <c r="A20" s="89"/>
       <c r="B20" s="83"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="138" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="129"/>
+      <c r="H20" s="83"/>
       <c r="I20" s="83"/>
       <c r="J20" s="83"/>
       <c r="K20" s="83"/>
@@ -13146,14 +13110,14 @@
     </row>
     <row r="21" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="83"/>
-      <c r="C21" s="134" t="s">
+      <c r="C21" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="139"/>
-      <c r="H21" s="129"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="83"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -13166,13 +13130,13 @@
     <row r="22" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="83"/>
       <c r="C22" s="95"/>
-      <c r="D22" s="141" t="s">
+      <c r="D22" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="E22" s="136"/>
-      <c r="F22" s="136"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="129"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="83"/>
       <c r="J22" s="83"/>
       <c r="K22" s="83"/>
@@ -13187,11 +13151,11 @@
       <c r="C23" s="51" t="s">
         <v>462</v>
       </c>
-      <c r="D23" s="142"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="129"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="83"/>
       <c r="I23" s="83"/>
       <c r="J23" s="83"/>
       <c r="K23" s="83"/>
@@ -13206,12 +13170,12 @@
       <c r="C24" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="134"/>
-      <c r="E24" s="138" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="F24" s="136"/>
-      <c r="G24" s="138"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="83"/>
       <c r="I24" s="83"/>
       <c r="J24" s="83"/>
@@ -13227,10 +13191,10 @@
       <c r="C25" s="23" t="s">
         <v>456</v>
       </c>
-      <c r="D25" s="134"/>
-      <c r="E25" s="139"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="83"/>
       <c r="I25" s="83"/>
       <c r="J25" s="83"/>
@@ -13244,19 +13208,19 @@
     <row r="26" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="83"/>
       <c r="C26" s="95"/>
-      <c r="D26" s="141" t="s">
+      <c r="D26" s="18" t="s">
         <v>467</v>
       </c>
-      <c r="E26" s="138"/>
-      <c r="F26" s="138"/>
-      <c r="G26" s="138"/>
-      <c r="H26" s="129"/>
-      <c r="I26" s="129"/>
-      <c r="J26" s="129"/>
-      <c r="K26" s="129"/>
-      <c r="L26" s="129"/>
-      <c r="M26" s="129"/>
-      <c r="N26" s="129"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="83"/>
+      <c r="L26" s="83"/>
+      <c r="M26" s="83"/>
+      <c r="N26" s="83"/>
       <c r="O26" s="83"/>
       <c r="P26" s="83"/>
     </row>
@@ -13265,36 +13229,36 @@
       <c r="C27" s="51" t="s">
         <v>455</v>
       </c>
-      <c r="D27" s="142"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="138"/>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="83"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="83"/>
+      <c r="M27" s="83"/>
+      <c r="N27" s="83"/>
       <c r="O27" s="83"/>
       <c r="P27" s="83"/>
     </row>
     <row r="28" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="83"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="136"/>
-      <c r="E28" s="136"/>
-      <c r="F28" s="138" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="G28" s="138"/>
-      <c r="H28" s="129"/>
-      <c r="I28" s="129"/>
-      <c r="J28" s="129"/>
-      <c r="K28" s="129"/>
-      <c r="L28" s="129"/>
-      <c r="M28" s="129"/>
-      <c r="N28" s="129"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="83"/>
+      <c r="J28" s="83"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="83"/>
+      <c r="M28" s="83"/>
+      <c r="N28" s="83"/>
       <c r="O28" s="83"/>
       <c r="P28" s="83"/>
     </row>
@@ -13303,36 +13267,36 @@
       <c r="C29" s="23" t="s">
         <v>457</v>
       </c>
-      <c r="D29" s="134"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="129"/>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
-      <c r="K29" s="129"/>
-      <c r="L29" s="129"/>
-      <c r="M29" s="129"/>
-      <c r="N29" s="129"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="83"/>
+      <c r="J29" s="83"/>
+      <c r="K29" s="83"/>
+      <c r="L29" s="83"/>
+      <c r="M29" s="83"/>
+      <c r="N29" s="83"/>
       <c r="O29" s="83"/>
       <c r="P29" s="83"/>
     </row>
     <row r="30" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="83"/>
       <c r="C30" s="95"/>
-      <c r="D30" s="141" t="s">
+      <c r="D30" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="E30" s="136"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="140"/>
-      <c r="H30" s="129"/>
-      <c r="I30" s="129"/>
-      <c r="J30" s="129"/>
-      <c r="K30" s="129"/>
-      <c r="L30" s="129"/>
-      <c r="M30" s="129"/>
-      <c r="N30" s="129"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="83"/>
+      <c r="M30" s="83"/>
+      <c r="N30" s="83"/>
       <c r="O30" s="83"/>
       <c r="P30" s="83"/>
     </row>
@@ -13341,36 +13305,36 @@
       <c r="C31" s="51" t="s">
         <v>458</v>
       </c>
-      <c r="D31" s="142"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="129"/>
-      <c r="I31" s="129"/>
-      <c r="J31" s="129"/>
-      <c r="K31" s="129"/>
-      <c r="L31" s="129"/>
-      <c r="M31" s="129"/>
-      <c r="N31" s="129"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
+      <c r="N31" s="83"/>
       <c r="O31" s="83"/>
       <c r="P31" s="83"/>
     </row>
     <row r="32" spans="1:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="83"/>
       <c r="C32" s="23"/>
-      <c r="D32" s="134"/>
-      <c r="E32" s="138" t="s">
+      <c r="D32" s="6"/>
+      <c r="E32" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="F32" s="138"/>
-      <c r="G32" s="140"/>
-      <c r="H32" s="129"/>
-      <c r="I32" s="129"/>
-      <c r="J32" s="129"/>
-      <c r="K32" s="129"/>
-      <c r="L32" s="129"/>
-      <c r="M32" s="129"/>
-      <c r="N32" s="129"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="83"/>
+      <c r="L32" s="83"/>
+      <c r="M32" s="83"/>
+      <c r="N32" s="83"/>
       <c r="O32" s="83"/>
       <c r="P32" s="83"/>
     </row>
@@ -13379,12 +13343,12 @@
       <c r="C33" s="23" t="s">
         <v>459</v>
       </c>
-      <c r="D33" s="134"/>
-      <c r="E33" s="139"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
       <c r="J33" s="83"/>
       <c r="K33" s="83"/>
       <c r="L33" s="83"/>
@@ -13396,75 +13360,75 @@
     <row r="34" spans="2:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="83"/>
       <c r="C34" s="95"/>
-      <c r="D34" s="141" t="s">
+      <c r="D34" s="18" t="s">
         <v>469</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="129"/>
-      <c r="G34" s="129"/>
-      <c r="H34" s="129"/>
-      <c r="I34" s="129"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
     </row>
     <row r="35" spans="2:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="83"/>
       <c r="C35" s="51" t="s">
         <v>460</v>
       </c>
-      <c r="D35" s="142"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="129"/>
-      <c r="G35" s="129"/>
-      <c r="H35" s="129"/>
-      <c r="I35" s="129"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
     </row>
     <row r="36" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B36" s="83"/>
-      <c r="C36" s="129"/>
-      <c r="D36" s="129"/>
-      <c r="E36" s="129"/>
-      <c r="F36" s="129"/>
-      <c r="G36" s="129"/>
-      <c r="H36" s="129"/>
-      <c r="I36" s="129"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37" s="129"/>
-      <c r="C37" s="129"/>
-      <c r="D37" s="129"/>
-      <c r="E37" s="129"/>
-      <c r="F37" s="129"/>
-      <c r="G37" s="129"/>
-      <c r="H37" s="129"/>
-      <c r="I37" s="129"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B38" s="129"/>
-      <c r="C38" s="129"/>
-      <c r="D38" s="129"/>
-      <c r="E38" s="129"/>
-      <c r="F38" s="129"/>
-      <c r="G38" s="129"/>
-      <c r="H38" s="129"/>
-      <c r="I38" s="129"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B39" s="129"/>
-      <c r="C39" s="129"/>
-      <c r="D39" s="129"/>
-      <c r="E39" s="129"/>
-      <c r="F39" s="129"/>
-      <c r="G39" s="129"/>
-      <c r="H39" s="129"/>
-      <c r="I39" s="129"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B40" s="129"/>
+      <c r="B40" s="83"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B41" s="129"/>
+      <c r="B41" s="83"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B42" s="129"/>
+      <c r="B42" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13496,16 +13460,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="115"/>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="111" t="s">
+      <c r="H5" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="112"/>
+      <c r="I5" s="115"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -17521,25 +17485,25 @@
     </row>
     <row r="2" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="115"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="124"/>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="113" t="s">
+      <c r="M2" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="115"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="124"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
@@ -17791,25 +17755,25 @@
     </row>
     <row r="10" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="113" t="s">
+      <c r="D10" s="122" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="115"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="124"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="113" t="s">
+      <c r="M10" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="114"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="115"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="123"/>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="123"/>
+      <c r="R10" s="124"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
@@ -19741,18 +19705,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="N11:P11"/>
-    <mergeCell ref="N12:P12"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="M2:R2"/>
     <mergeCell ref="D10:I10"/>
@@ -19769,6 +19721,18 @@
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20393,26 +20357,26 @@
     </row>
     <row r="2" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="115"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="124"/>
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="113" t="s">
+      <c r="N2" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="115"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="124"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
@@ -20432,7 +20396,7 @@
       <c r="I3" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="123"/>
+      <c r="J3" s="125"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="1"/>
@@ -20469,7 +20433,7 @@
       <c r="I4" s="116">
         <v>0</v>
       </c>
-      <c r="J4" s="123"/>
+      <c r="J4" s="125"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="1"/>
@@ -20506,7 +20470,7 @@
       <c r="I5" s="116">
         <v>1</v>
       </c>
-      <c r="J5" s="123"/>
+      <c r="J5" s="125"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
       <c r="M5" s="1"/>
@@ -20543,7 +20507,7 @@
       <c r="I6" s="116">
         <v>2</v>
       </c>
-      <c r="J6" s="123"/>
+      <c r="J6" s="125"/>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
       <c r="M6" s="1"/>
@@ -20580,7 +20544,7 @@
       <c r="I7" s="116">
         <v>3</v>
       </c>
-      <c r="J7" s="123"/>
+      <c r="J7" s="125"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="1"/>
@@ -20617,7 +20581,7 @@
       <c r="I8" s="116">
         <v>4</v>
       </c>
-      <c r="J8" s="123"/>
+      <c r="J8" s="125"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
       <c r="M8" s="1"/>
@@ -20654,7 +20618,7 @@
       <c r="I9" s="119">
         <v>5</v>
       </c>
-      <c r="J9" s="124"/>
+      <c r="J9" s="126"/>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
       <c r="M9" s="1"/>
@@ -22460,12 +22424,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="E6:G6"/>
@@ -22475,14 +22441,12 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="O9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23245,12 +23209,12 @@
       <c r="H13">
         <v>3</v>
       </c>
-      <c r="T13" s="125" t="s">
+      <c r="T13" s="128" t="s">
         <v>118</v>
       </c>
-      <c r="U13" s="125"/>
-      <c r="V13" s="125"/>
-      <c r="W13" s="125"/>
+      <c r="U13" s="128"/>
+      <c r="V13" s="128"/>
+      <c r="W13" s="128"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -41578,7 +41542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C010E2E9-5FD8-4977-AB68-FE330F0CC9E1}">
   <dimension ref="A3:DD40"/>
   <sheetViews>
-    <sheetView topLeftCell="BD4" workbookViewId="0">
+    <sheetView topLeftCell="AC4" workbookViewId="0">
       <selection activeCell="BR32" sqref="BR32"/>
     </sheetView>
   </sheetViews>
@@ -41750,8 +41714,8 @@
       <c r="F5" s="83"/>
       <c r="G5" s="1"/>
       <c r="H5" s="59"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="6" t="s">
         <v>373</v>
       </c>
@@ -41888,8 +41852,8 @@
       <c r="F6" s="83"/>
       <c r="G6" s="1"/>
       <c r="H6" s="59"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="64"/>
       <c r="L6" s="60" t="s">
         <v>8</v>
@@ -42032,8 +41996,8 @@
       <c r="F7" s="83"/>
       <c r="G7" s="1"/>
       <c r="H7" s="59"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="12" t="s">
         <v>374</v>
       </c>
@@ -42162,7 +42126,7 @@
     <row r="8" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="83"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="131"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="61" t="s">
         <v>12</v>
       </c>
@@ -42170,12 +42134,12 @@
       <c r="F8" s="83"/>
       <c r="G8" s="1"/>
       <c r="H8" s="59"/>
-      <c r="I8" s="128"/>
-      <c r="J8" s="128"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="131"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="61"/>
-      <c r="N8" s="130" t="s">
+      <c r="N8" s="61" t="s">
         <v>12</v>
       </c>
       <c r="O8" s="5" t="s">
@@ -42185,7 +42149,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="23"/>
-      <c r="T8" s="131"/>
+      <c r="T8" s="6"/>
       <c r="U8" s="61" t="s">
         <v>12</v>
       </c>
@@ -42193,9 +42157,9 @@
       <c r="W8" s="83"/>
       <c r="X8" s="83"/>
       <c r="Y8" s="23"/>
-      <c r="Z8" s="131"/>
+      <c r="Z8" s="6"/>
       <c r="AA8" s="61"/>
-      <c r="AB8" s="130" t="s">
+      <c r="AB8" s="61" t="s">
         <v>12</v>
       </c>
       <c r="AC8" s="93"/>
@@ -42203,9 +42167,9 @@
       <c r="AE8" s="83"/>
       <c r="AF8" s="1"/>
       <c r="AG8" s="23"/>
-      <c r="AH8" s="131"/>
+      <c r="AH8" s="6"/>
       <c r="AI8" s="61"/>
-      <c r="AJ8" s="130" t="s">
+      <c r="AJ8" s="61" t="s">
         <v>12</v>
       </c>
       <c r="AK8" s="93"/>
@@ -42232,7 +42196,7 @@
       <c r="AZ8" s="1"/>
       <c r="BA8" s="59"/>
       <c r="BB8" s="6"/>
-      <c r="BC8" s="131"/>
+      <c r="BC8" s="6"/>
       <c r="BD8" s="61" t="s">
         <v>12</v>
       </c>
@@ -42243,7 +42207,7 @@
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
       <c r="BI8" s="23"/>
-      <c r="BJ8" s="132"/>
+      <c r="BJ8" s="23"/>
       <c r="BK8" s="61" t="s">
         <v>12</v>
       </c>
@@ -42259,7 +42223,7 @@
       <c r="BS8" s="83"/>
       <c r="BT8" s="1"/>
       <c r="BU8" s="23"/>
-      <c r="BV8" s="132"/>
+      <c r="BV8" s="23"/>
       <c r="BW8" s="61" t="s">
         <v>12</v>
       </c>
@@ -42308,20 +42272,20 @@
       <c r="B9" s="23">
         <v>4</v>
       </c>
-      <c r="C9" s="131"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="83"/>
       <c r="E9" s="92"/>
       <c r="F9" s="93"/>
       <c r="G9" s="1"/>
       <c r="H9" s="59"/>
-      <c r="I9" s="128"/>
-      <c r="J9" s="128"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="L9" s="131"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="128"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="1"/>
@@ -42329,17 +42293,17 @@
       <c r="S9" s="23">
         <v>4</v>
       </c>
-      <c r="T9" s="131"/>
+      <c r="T9" s="6"/>
       <c r="U9" s="83"/>
       <c r="V9" s="92"/>
       <c r="W9" s="93"/>
-      <c r="X9" s="129"/>
+      <c r="X9" s="83"/>
       <c r="Y9" s="23">
         <v>4</v>
       </c>
-      <c r="Z9" s="131"/>
+      <c r="Z9" s="6"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="128"/>
+      <c r="AB9" s="1"/>
       <c r="AC9" s="92"/>
       <c r="AD9" s="93"/>
       <c r="AE9" s="83"/>
@@ -42347,9 +42311,9 @@
       <c r="AG9" s="23">
         <v>4</v>
       </c>
-      <c r="AH9" s="131"/>
+      <c r="AH9" s="6"/>
       <c r="AI9" s="1"/>
-      <c r="AJ9" s="128"/>
+      <c r="AJ9" s="1"/>
       <c r="AK9" s="92"/>
       <c r="AL9" s="93"/>
       <c r="AM9" s="83"/>
@@ -42374,7 +42338,7 @@
       <c r="BB9" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="BC9" s="131"/>
+      <c r="BC9" s="6"/>
       <c r="BD9" s="1"/>
       <c r="BE9" s="4"/>
       <c r="BF9" s="5"/>
@@ -42383,7 +42347,7 @@
       <c r="BI9" s="23">
         <v>4</v>
       </c>
-      <c r="BJ9" s="132"/>
+      <c r="BJ9" s="23"/>
       <c r="BK9" s="83"/>
       <c r="BL9" s="92"/>
       <c r="BM9" s="93"/>
@@ -42399,7 +42363,7 @@
       <c r="BU9" s="23">
         <v>4</v>
       </c>
-      <c r="BV9" s="132"/>
+      <c r="BV9" s="23"/>
       <c r="BW9" s="83"/>
       <c r="BX9" s="92"/>
       <c r="BY9" s="93"/>
@@ -42452,8 +42416,8 @@
       <c r="F10" s="93"/>
       <c r="G10" s="1"/>
       <c r="H10" s="59"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="64"/>
       <c r="L10" s="60" t="s">
         <v>9</v>
@@ -42461,7 +42425,7 @@
       <c r="M10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="128"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="1"/>
@@ -42473,13 +42437,13 @@
       <c r="U10" s="83"/>
       <c r="V10" s="93"/>
       <c r="W10" s="93"/>
-      <c r="X10" s="129"/>
+      <c r="X10" s="83"/>
       <c r="Y10" s="64"/>
       <c r="Z10" s="60" t="s">
         <v>9</v>
       </c>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="128"/>
+      <c r="AB10" s="1"/>
       <c r="AC10" s="93"/>
       <c r="AD10" s="93"/>
       <c r="AE10" s="83"/>
@@ -42489,7 +42453,7 @@
         <v>9</v>
       </c>
       <c r="AI10" s="1"/>
-      <c r="AJ10" s="128"/>
+      <c r="AJ10" s="1"/>
       <c r="AK10" s="93"/>
       <c r="AL10" s="93"/>
       <c r="AM10" s="83"/>
@@ -42596,8 +42560,8 @@
       <c r="F11" s="93"/>
       <c r="G11" s="1"/>
       <c r="H11" s="59"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="12" t="s">
         <v>376</v>
       </c>
@@ -42615,7 +42579,7 @@
       <c r="U11" s="92"/>
       <c r="V11" s="83"/>
       <c r="W11" s="93"/>
-      <c r="X11" s="129"/>
+      <c r="X11" s="83"/>
       <c r="Y11" s="51">
         <v>5</v>
       </c>
@@ -42726,7 +42690,7 @@
     <row r="12" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="83"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="131"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="83"/>
       <c r="E12" s="61" t="s">
         <v>14</v>
@@ -42734,12 +42698,12 @@
       <c r="F12" s="93"/>
       <c r="G12" s="1"/>
       <c r="H12" s="59"/>
-      <c r="I12" s="128"/>
-      <c r="J12" s="128"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="131"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="128"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="61" t="s">
         <v>14</v>
       </c>
@@ -42749,17 +42713,17 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="23"/>
-      <c r="T12" s="131"/>
+      <c r="T12" s="6"/>
       <c r="U12" s="83"/>
       <c r="V12" s="61" t="s">
         <v>14</v>
       </c>
       <c r="W12" s="93"/>
-      <c r="X12" s="129"/>
+      <c r="X12" s="83"/>
       <c r="Y12" s="23"/>
-      <c r="Z12" s="131"/>
+      <c r="Z12" s="6"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="128"/>
+      <c r="AB12" s="1"/>
       <c r="AC12" s="61" t="s">
         <v>14</v>
       </c>
@@ -42767,9 +42731,9 @@
       <c r="AE12" s="83"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="23"/>
-      <c r="AH12" s="131"/>
+      <c r="AH12" s="6"/>
       <c r="AI12" s="1"/>
-      <c r="AJ12" s="128"/>
+      <c r="AJ12" s="1"/>
       <c r="AK12" s="61" t="s">
         <v>14</v>
       </c>
@@ -42796,7 +42760,7 @@
       <c r="AZ12" s="1"/>
       <c r="BA12" s="59"/>
       <c r="BB12" s="6"/>
-      <c r="BC12" s="131"/>
+      <c r="BC12" s="6"/>
       <c r="BD12" s="1"/>
       <c r="BE12" s="61" t="s">
         <v>14</v>
@@ -42807,7 +42771,7 @@
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="23"/>
-      <c r="BJ12" s="132"/>
+      <c r="BJ12" s="23"/>
       <c r="BK12" s="83"/>
       <c r="BL12" s="61" t="s">
         <v>14</v>
@@ -42823,7 +42787,7 @@
       <c r="BS12" s="83"/>
       <c r="BT12" s="1"/>
       <c r="BU12" s="23"/>
-      <c r="BV12" s="132"/>
+      <c r="BV12" s="23"/>
       <c r="BW12" s="83"/>
       <c r="BX12" s="61" t="s">
         <v>14</v>
@@ -42870,20 +42834,20 @@
       <c r="B13" s="23">
         <v>3</v>
       </c>
-      <c r="C13" s="131"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="83"/>
       <c r="E13" s="83"/>
       <c r="F13" s="92"/>
       <c r="G13" s="1"/>
       <c r="H13" s="59"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="128"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="L13" s="131"/>
+      <c r="L13" s="6"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="128"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
@@ -42891,17 +42855,17 @@
       <c r="S13" s="23">
         <v>3</v>
       </c>
-      <c r="T13" s="131"/>
+      <c r="T13" s="6"/>
       <c r="U13" s="83"/>
       <c r="V13" s="83"/>
       <c r="W13" s="92"/>
-      <c r="X13" s="129"/>
+      <c r="X13" s="83"/>
       <c r="Y13" s="23">
         <v>3</v>
       </c>
-      <c r="Z13" s="131"/>
+      <c r="Z13" s="6"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="128"/>
+      <c r="AB13" s="1"/>
       <c r="AC13" s="83"/>
       <c r="AD13" s="92"/>
       <c r="AE13" s="83"/>
@@ -42909,9 +42873,9 @@
       <c r="AG13" s="23">
         <v>3</v>
       </c>
-      <c r="AH13" s="131"/>
+      <c r="AH13" s="6"/>
       <c r="AI13" s="1"/>
-      <c r="AJ13" s="128"/>
+      <c r="AJ13" s="1"/>
       <c r="AK13" s="83"/>
       <c r="AL13" s="92"/>
       <c r="AM13" s="83"/>
@@ -42936,7 +42900,7 @@
       <c r="BB13" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="BC13" s="131"/>
+      <c r="BC13" s="6"/>
       <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
       <c r="BF13" s="4"/>
@@ -42945,7 +42909,7 @@
       <c r="BI13" s="23">
         <v>3</v>
       </c>
-      <c r="BJ13" s="132"/>
+      <c r="BJ13" s="23"/>
       <c r="BK13" s="83"/>
       <c r="BL13" s="83"/>
       <c r="BM13" s="92"/>
@@ -42961,7 +42925,7 @@
       <c r="BU13" s="23">
         <v>3</v>
       </c>
-      <c r="BV13" s="132"/>
+      <c r="BV13" s="23"/>
       <c r="BW13" s="83"/>
       <c r="BX13" s="83"/>
       <c r="BY13" s="92"/>
@@ -43014,8 +42978,8 @@
       <c r="F14" s="93"/>
       <c r="G14" s="1"/>
       <c r="H14" s="59"/>
-      <c r="I14" s="128"/>
-      <c r="J14" s="128"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="64"/>
       <c r="L14" s="60" t="s">
         <v>10</v>
@@ -43023,7 +42987,7 @@
       <c r="M14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="128"/>
+      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="1"/>
@@ -43035,13 +42999,13 @@
       <c r="U14" s="83"/>
       <c r="V14" s="83"/>
       <c r="W14" s="93"/>
-      <c r="X14" s="129"/>
+      <c r="X14" s="83"/>
       <c r="Y14" s="64"/>
       <c r="Z14" s="60" t="s">
         <v>10</v>
       </c>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="128"/>
+      <c r="AB14" s="1"/>
       <c r="AC14" s="83"/>
       <c r="AD14" s="93"/>
       <c r="AE14" s="83"/>
@@ -43051,7 +43015,7 @@
         <v>10</v>
       </c>
       <c r="AI14" s="1"/>
-      <c r="AJ14" s="128"/>
+      <c r="AJ14" s="1"/>
       <c r="AK14" s="83"/>
       <c r="AL14" s="93"/>
       <c r="AM14" s="83"/>
@@ -43158,8 +43122,8 @@
       <c r="F15" s="93"/>
       <c r="G15" s="1"/>
       <c r="H15" s="59"/>
-      <c r="I15" s="128"/>
-      <c r="J15" s="128"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="12" t="s">
         <v>378</v>
       </c>
@@ -43177,7 +43141,7 @@
       <c r="U15" s="92"/>
       <c r="V15" s="93"/>
       <c r="W15" s="93"/>
-      <c r="X15" s="129"/>
+      <c r="X15" s="83"/>
       <c r="Y15" s="51">
         <v>6</v>
       </c>
@@ -43288,7 +43252,7 @@
     <row r="16" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="83"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="131"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="61" t="s">
         <v>13</v>
       </c>
@@ -43296,12 +43260,12 @@
       <c r="F16" s="93"/>
       <c r="G16" s="1"/>
       <c r="H16" s="59"/>
-      <c r="I16" s="128"/>
-      <c r="J16" s="128"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="131"/>
+      <c r="L16" s="6"/>
       <c r="M16" s="61"/>
-      <c r="N16" s="130" t="s">
+      <c r="N16" s="61" t="s">
         <v>13</v>
       </c>
       <c r="O16" s="5" t="s">
@@ -43311,17 +43275,17 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="23"/>
-      <c r="T16" s="131"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="61" t="s">
         <v>13</v>
       </c>
       <c r="V16" s="93"/>
       <c r="W16" s="93"/>
-      <c r="X16" s="129"/>
+      <c r="X16" s="83"/>
       <c r="Y16" s="23"/>
-      <c r="Z16" s="131"/>
+      <c r="Z16" s="6"/>
       <c r="AA16" s="61"/>
-      <c r="AB16" s="130" t="s">
+      <c r="AB16" s="61" t="s">
         <v>13</v>
       </c>
       <c r="AC16" s="93"/>
@@ -43329,9 +43293,9 @@
       <c r="AE16" s="83"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="23"/>
-      <c r="AH16" s="131"/>
+      <c r="AH16" s="6"/>
       <c r="AI16" s="61"/>
-      <c r="AJ16" s="130" t="s">
+      <c r="AJ16" s="61" t="s">
         <v>13</v>
       </c>
       <c r="AK16" s="93"/>
@@ -43358,7 +43322,7 @@
       <c r="AZ16" s="1"/>
       <c r="BA16" s="59"/>
       <c r="BB16" s="6"/>
-      <c r="BC16" s="131"/>
+      <c r="BC16" s="6"/>
       <c r="BD16" s="61" t="s">
         <v>13</v>
       </c>
@@ -43369,7 +43333,7 @@
       <c r="BG16" s="1"/>
       <c r="BH16" s="1"/>
       <c r="BI16" s="23"/>
-      <c r="BJ16" s="132"/>
+      <c r="BJ16" s="23"/>
       <c r="BK16" s="61" t="s">
         <v>13</v>
       </c>
@@ -43385,7 +43349,7 @@
       <c r="BS16" s="83"/>
       <c r="BT16" s="1"/>
       <c r="BU16" s="23"/>
-      <c r="BV16" s="132"/>
+      <c r="BV16" s="23"/>
       <c r="BW16" s="61" t="s">
         <v>13</v>
       </c>
@@ -43434,20 +43398,20 @@
       <c r="B17" s="23">
         <v>2</v>
       </c>
-      <c r="C17" s="131"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="83"/>
       <c r="E17" s="92"/>
       <c r="F17" s="83"/>
       <c r="G17" s="1"/>
       <c r="H17" s="59"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="128"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="L17" s="131"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="128"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="4"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -43455,7 +43419,7 @@
       <c r="S17" s="23">
         <v>2</v>
       </c>
-      <c r="T17" s="131"/>
+      <c r="T17" s="6"/>
       <c r="U17" s="83"/>
       <c r="V17" s="92"/>
       <c r="W17" s="83"/>
@@ -43463,9 +43427,9 @@
       <c r="Y17" s="23">
         <v>2</v>
       </c>
-      <c r="Z17" s="131"/>
+      <c r="Z17" s="6"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="128"/>
+      <c r="AB17" s="1"/>
       <c r="AC17" s="92"/>
       <c r="AD17" s="83"/>
       <c r="AE17" s="83"/>
@@ -43473,9 +43437,9 @@
       <c r="AG17" s="23">
         <v>2</v>
       </c>
-      <c r="AH17" s="131"/>
+      <c r="AH17" s="6"/>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="128"/>
+      <c r="AJ17" s="1"/>
       <c r="AK17" s="92"/>
       <c r="AL17" s="83"/>
       <c r="AM17" s="83"/>
@@ -43500,7 +43464,7 @@
       <c r="BB17" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="BC17" s="131"/>
+      <c r="BC17" s="6"/>
       <c r="BD17" s="1"/>
       <c r="BE17" s="4"/>
       <c r="BF17" s="1"/>
@@ -43509,7 +43473,7 @@
       <c r="BI17" s="23">
         <v>2</v>
       </c>
-      <c r="BJ17" s="132"/>
+      <c r="BJ17" s="23"/>
       <c r="BK17" s="83"/>
       <c r="BL17" s="92"/>
       <c r="BM17" s="83"/>
@@ -43525,7 +43489,7 @@
       <c r="BU17" s="23">
         <v>2</v>
       </c>
-      <c r="BV17" s="132"/>
+      <c r="BV17" s="23"/>
       <c r="BW17" s="83"/>
       <c r="BX17" s="92"/>
       <c r="BY17" s="83"/>
@@ -43578,8 +43542,8 @@
       <c r="F18" s="83"/>
       <c r="G18" s="1"/>
       <c r="H18" s="59"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="128"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="64"/>
       <c r="L18" s="60" t="s">
         <v>11</v>
@@ -43587,7 +43551,7 @@
       <c r="M18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N18" s="128"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="5"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -43601,13 +43565,13 @@
       <c r="W18" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="X18" s="129"/>
+      <c r="X18" s="83"/>
       <c r="Y18" s="64"/>
       <c r="Z18" s="60" t="s">
         <v>11</v>
       </c>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="128"/>
+      <c r="AB18" s="1"/>
       <c r="AC18" s="93"/>
       <c r="AD18" s="83"/>
       <c r="AE18" s="83"/>
@@ -43617,7 +43581,7 @@
         <v>11</v>
       </c>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="128"/>
+      <c r="AJ18" s="1"/>
       <c r="AK18" s="93"/>
       <c r="AL18" s="83"/>
       <c r="AM18" s="83"/>
@@ -43728,8 +43692,8 @@
       <c r="F19" s="83"/>
       <c r="G19" s="1"/>
       <c r="H19" s="59"/>
-      <c r="I19" s="128"/>
-      <c r="J19" s="128"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="12" t="s">
         <v>380</v>
       </c>
@@ -43872,12 +43836,12 @@
       <c r="F20" s="83"/>
       <c r="G20" s="1"/>
       <c r="H20" s="59"/>
-      <c r="I20" s="128"/>
-      <c r="J20" s="128"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="128"/>
+      <c r="N20" s="1"/>
       <c r="O20" s="6" t="s">
         <v>381</v>
       </c>
@@ -43895,7 +43859,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
-      <c r="AB20" s="128"/>
+      <c r="AB20" s="1"/>
       <c r="AC20" s="23" t="s">
         <v>12</v>
       </c>
@@ -43907,7 +43871,7 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
-      <c r="AJ20" s="128"/>
+      <c r="AJ20" s="1"/>
       <c r="AK20" s="23" t="s">
         <v>12</v>
       </c>
@@ -43943,7 +43907,7 @@
       <c r="BG20" s="1"/>
       <c r="BH20" s="1"/>
       <c r="BI20" s="83"/>
-      <c r="BJ20" s="129"/>
+      <c r="BJ20" s="83"/>
       <c r="BK20" s="83"/>
       <c r="BL20" s="23" t="s">
         <v>13</v>
@@ -43959,7 +43923,7 @@
       <c r="BS20" s="83"/>
       <c r="BT20" s="1"/>
       <c r="BU20" s="83"/>
-      <c r="BV20" s="129"/>
+      <c r="BV20" s="83"/>
       <c r="BW20" s="83"/>
       <c r="BX20" s="23" t="s">
         <v>13</v>
@@ -44014,8 +43978,8 @@
       <c r="F21" s="83"/>
       <c r="G21" s="1"/>
       <c r="H21" s="59"/>
-      <c r="I21" s="128"/>
-      <c r="J21" s="128"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -44174,8 +44138,8 @@
       <c r="F22" s="92"/>
       <c r="G22" s="1"/>
       <c r="H22" s="59"/>
-      <c r="I22" s="128"/>
-      <c r="J22" s="128"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -44193,7 +44157,7 @@
         <v>13</v>
       </c>
       <c r="W22" s="92"/>
-      <c r="X22" s="129"/>
+      <c r="X22" s="83"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
@@ -44314,8 +44278,8 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="59"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -44449,7 +44413,7 @@
     </row>
     <row r="24" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="83" t="s">
         <v>383</v>
       </c>
       <c r="C24" s="83" t="s">
@@ -44460,9 +44424,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="59"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="128"/>
-      <c r="K24" s="129" t="s">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="83" t="s">
         <v>383</v>
       </c>
       <c r="L24" s="83" t="s">
@@ -44476,13 +44440,13 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="129"/>
+      <c r="S24" s="83"/>
       <c r="T24" s="83"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="129"/>
+      <c r="Y24" s="83"/>
       <c r="Z24" s="83"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -44490,7 +44454,7 @@
       <c r="AD24" s="83"/>
       <c r="AE24" s="83"/>
       <c r="AF24" s="1"/>
-      <c r="AG24" s="129" t="s">
+      <c r="AG24" s="83" t="s">
         <v>383</v>
       </c>
       <c r="AH24" s="83" t="s">
@@ -44591,7 +44555,7 @@
     </row>
     <row r="25" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="129" t="s">
+      <c r="B25" s="83" t="s">
         <v>384</v>
       </c>
       <c r="C25" s="83" t="s">
@@ -44602,9 +44566,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="59"/>
-      <c r="I25" s="128"/>
-      <c r="J25" s="128"/>
-      <c r="K25" s="129" t="s">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="83" t="s">
         <v>384</v>
       </c>
       <c r="L25" s="83" t="s">
@@ -44618,13 +44582,13 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="129"/>
+      <c r="S25" s="83"/>
       <c r="T25" s="83"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="129"/>
+      <c r="Y25" s="83"/>
       <c r="Z25" s="83"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -44632,7 +44596,7 @@
       <c r="AD25" s="83"/>
       <c r="AE25" s="83"/>
       <c r="AF25" s="1"/>
-      <c r="AG25" s="129" t="s">
+      <c r="AG25" s="83" t="s">
         <v>384</v>
       </c>
       <c r="AH25" s="83" t="s">
@@ -44751,7 +44715,7 @@
     </row>
     <row r="26" spans="1:108" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="83" t="s">
         <v>385</v>
       </c>
       <c r="C26" s="83" t="s">
@@ -44762,9 +44726,9 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="59"/>
-      <c r="I26" s="128"/>
-      <c r="J26" s="128"/>
-      <c r="K26" s="129" t="s">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="83" t="s">
         <v>385</v>
       </c>
       <c r="L26" s="83" t="s">
@@ -44778,13 +44742,13 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="129"/>
+      <c r="S26" s="83"/>
       <c r="T26" s="83"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
-      <c r="Y26" s="129"/>
+      <c r="Y26" s="83"/>
       <c r="Z26" s="83"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
@@ -44792,7 +44756,7 @@
       <c r="AD26" s="83"/>
       <c r="AE26" s="83"/>
       <c r="AF26" s="1"/>
-      <c r="AG26" s="129" t="s">
+      <c r="AG26" s="83" t="s">
         <v>385</v>
       </c>
       <c r="AH26" s="83" t="s">
@@ -44904,8 +44868,8 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="128"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -45149,7 +45113,7 @@
       <c r="AY29" s="1"/>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="59"/>
-      <c r="BB29" s="129" t="s">
+      <c r="BB29" s="83" t="s">
         <v>383</v>
       </c>
       <c r="BC29" s="83" t="s">
@@ -45162,7 +45126,7 @@
       <c r="BF29" s="1"/>
       <c r="BG29" s="1"/>
       <c r="BH29" s="1"/>
-      <c r="BI29" s="129" t="s">
+      <c r="BI29" s="83" t="s">
         <v>383</v>
       </c>
       <c r="BJ29" s="83" t="s">
@@ -45172,7 +45136,7 @@
       <c r="BL29" s="1"/>
       <c r="BM29" s="1"/>
       <c r="BN29" s="1"/>
-      <c r="BU29" s="129"/>
+      <c r="BU29" s="83"/>
       <c r="BV29" s="83"/>
       <c r="BW29" s="1"/>
       <c r="BX29" s="1"/>
@@ -45197,7 +45161,7 @@
       <c r="AY30" s="1"/>
       <c r="AZ30" s="1"/>
       <c r="BA30" s="59"/>
-      <c r="BB30" s="129" t="s">
+      <c r="BB30" s="83" t="s">
         <v>384</v>
       </c>
       <c r="BC30" s="83" t="s">
@@ -45210,7 +45174,7 @@
       <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
       <c r="BH30" s="1"/>
-      <c r="BI30" s="129" t="s">
+      <c r="BI30" s="83" t="s">
         <v>384</v>
       </c>
       <c r="BJ30" s="83" t="s">
@@ -45220,7 +45184,7 @@
       <c r="BL30" s="1"/>
       <c r="BM30" s="1"/>
       <c r="BN30" s="1"/>
-      <c r="BU30" s="129"/>
+      <c r="BU30" s="83"/>
       <c r="BV30" s="83"/>
       <c r="BW30" s="1"/>
       <c r="BX30" s="1"/>
@@ -45247,7 +45211,7 @@
       <c r="AY31" s="1"/>
       <c r="AZ31" s="1"/>
       <c r="BA31" s="59"/>
-      <c r="BB31" s="129" t="s">
+      <c r="BB31" s="83" t="s">
         <v>385</v>
       </c>
       <c r="BC31" s="83" t="s">
@@ -45260,7 +45224,7 @@
       <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
-      <c r="BI31" s="129" t="s">
+      <c r="BI31" s="83" t="s">
         <v>408</v>
       </c>
       <c r="BJ31" s="83" t="s">
@@ -45270,7 +45234,7 @@
       <c r="BL31" s="1"/>
       <c r="BM31" s="1"/>
       <c r="BN31" s="1"/>
-      <c r="BU31" s="129"/>
+      <c r="BU31" s="83"/>
       <c r="BV31" s="83"/>
       <c r="BW31" s="1"/>
       <c r="BX31" s="1"/>
@@ -45297,7 +45261,7 @@
       <c r="AY32" s="1"/>
       <c r="AZ32" s="1"/>
       <c r="BA32" s="59"/>
-      <c r="BB32" s="129" t="s">
+      <c r="BB32" s="83" t="s">
         <v>408</v>
       </c>
       <c r="BC32" s="83" t="s">
@@ -46222,20 +46186,20 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="126" t="s">
+      <c r="F33" s="129" t="s">
         <v>174</v>
       </c>
-      <c r="G33" s="126"/>
+      <c r="G33" s="129"/>
       <c r="H33" s="1"/>
       <c r="I33" s="59"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="133" t="s">
+      <c r="N33" s="130" t="s">
         <v>174</v>
       </c>
-      <c r="O33" s="133"/>
+      <c r="O33" s="130"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
@@ -46245,16 +46209,16 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="126"/>
-      <c r="G34" s="126"/>
+      <c r="F34" s="129"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="1"/>
       <c r="I34" s="59"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="133"/>
-      <c r="O34" s="133"/>
+      <c r="N34" s="130"/>
+      <c r="O34" s="130"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
@@ -46661,8 +46625,8 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="126"/>
-      <c r="G53" s="126"/>
+      <c r="F53" s="129"/>
+      <c r="G53" s="129"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1" t="s">
@@ -46671,24 +46635,24 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="126"/>
-      <c r="O53" s="126"/>
+      <c r="N53" s="129"/>
+      <c r="O53" s="129"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="126"/>
-      <c r="G54" s="126"/>
+      <c r="F54" s="129"/>
+      <c r="G54" s="129"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="126"/>
-      <c r="O54" s="126"/>
+      <c r="N54" s="129"/>
+      <c r="O54" s="129"/>
     </row>
     <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I55" s="1"/>
@@ -50957,8 +50921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC45635-DE39-4CBA-B2B1-B5066770F06C}">
   <dimension ref="B1:Y50"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51665,7 +51629,7 @@
       <c r="I22" s="83"/>
       <c r="J22" s="83"/>
       <c r="K22" s="23" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="L22" s="83"/>
       <c r="M22" s="1"/>
@@ -69792,7 +69756,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ4 BZ6 BZ8 BZ10 BZ12 BZ14 BZ16 BZ18 BZ20 BZ22 BZ24 BZ26 BZ28 BZ30 BZ32 BZ34 BZ36 BZ38 BZ40 BZ42 BZ44 BZ46 BZ48 BZ50 BZ52 BZ54 BZ56 BZ58 BZ60 BZ62 BZ64 BZ66 BZ68 BZ70 BZ72 BZ74 BZ76 BZ78 BZ80 BZ82 BZ84 BZ86 BZ88 BZ90 BZ92 BZ94 BZ96 BZ98 BZ100 BZ102 BZ104">
+  <conditionalFormatting sqref="BZ6 BZ4 BZ8 BZ10 BZ12 BZ14 BZ16 BZ18 BZ20 BZ22 BZ24 BZ26 BZ28 BZ30 BZ32 BZ34 BZ36 BZ38 BZ40 BZ42 BZ44 BZ46 BZ48 BZ50 BZ52 BZ54 BZ56 BZ58 BZ60 BZ62 BZ64 BZ66 BZ68 BZ70 BZ72 BZ74 BZ76 BZ78 BZ80 BZ82 BZ84 BZ86 BZ88 BZ90 BZ92 BZ94 BZ96 BZ98 BZ100 BZ102 BZ104">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -69804,7 +69768,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA4 CA6 CA8 CA10 CA12 CA14 CA16 CA18 CA20 CA22 CA24 CA26 CA28 CA30 CA32 CA34 CA36 CA38 CA40 CA42 CA44 CA46 CA48 CA50 CA52 CA54 CA56 CA58 CA60 CA62 CA64 CA66 CA68 CA70 CA72 CA74 CA76 CA78 CA80 CA82 CA84 CA86 CA88 CA90 CA92 CA94 CA96 CA98 CA100 CA102 CA104">
+  <conditionalFormatting sqref="CA6 CA4 CA8 CA10 CA12 CA14 CA16 CA18 CA20 CA22 CA24 CA26 CA28 CA30 CA32 CA34 CA36 CA38 CA40 CA42 CA44 CA46 CA48 CA50 CA52 CA54 CA56 CA58 CA60 CA62 CA64 CA66 CA68 CA70 CA72 CA74 CA76 CA78 CA80 CA82 CA84 CA86 CA88 CA90 CA92 CA94 CA96 CA98 CA100 CA102 CA104">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -69816,7 +69780,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CB4 CB6 CB8 CB10 CB12 CB14 CB16 CB18 CB20 CB22 CB24 CB26 CB28 CB30 CB32 CB34 CB36 CB38 CB40 CB42 CB44 CB46 CB48 CB50 CB52 CB54 CB56 CB58 CB60 CB62 CB64 CB66 CB68 CB70 CB72 CB74 CB76 CB78 CB80 CB82 CB84 CB86 CB88 CB90 CB92 CB94 CB96 CB98 CB100 CB102 CB104">
+  <conditionalFormatting sqref="CB6 CB4 CB8 CB10 CB12 CB14 CB16 CB18 CB20 CB22 CB24 CB26 CB28 CB30 CB32 CB34 CB36 CB38 CB40 CB42 CB44 CB46 CB48 CB50 CB52 CB54 CB56 CB58 CB60 CB62 CB64 CB66 CB68 CB70 CB72 CB74 CB76 CB78 CB80 CB82 CB84 CB86 CB88 CB90 CB92 CB94 CB96 CB98 CB100 CB102 CB104">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -69828,7 +69792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CC4 CC6 CC8 CC10 CC12 CC14 CC16 CC18 CC20 CC22 CC24 CC26 CC28 CC30 CC32 CC34 CC36 CC38 CC40 CC42 CC44 CC46 CC48 CC50 CC52 CC54 CC56 CC58 CC60 CC62 CC64 CC66 CC68 CC70 CC72 CC74 CC76 CC78 CC80 CC82 CC84 CC86 CC88 CC90 CC92 CC94 CC96 CC98 CC100 CC102 CC104">
+  <conditionalFormatting sqref="CC6 CC4 CC8 CC10 CC12 CC14 CC16 CC18 CC20 CC22 CC24 CC26 CC28 CC30 CC32 CC34 CC36 CC38 CC40 CC42 CC44 CC46 CC48 CC50 CC52 CC54 CC56 CC58 CC60 CC62 CC64 CC66 CC68 CC70 CC72 CC74 CC76 CC78 CC80 CC82 CC84 CC86 CC88 CC90 CC92 CC94 CC96 CC98 CC100 CC102 CC104">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -69840,7 +69804,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CD4 CD6 CD8 CD10 CD12 CD14 CD16 CD18 CD20 CD22 CD24 CD26 CD28 CD30 CD32 CD34 CD36 CD38 CD40 CD42 CD44 CD46 CD48 CD50 CD52 CD54 CD56 CD58 CD60 CD62 CD64 CD66 CD68 CD70 CD72 CD74 CD76 CD78 CD80 CD82 CD84 CD86 CD88 CD90 CD92 CD94 CD96 CD98 CD100 CD102 CD104">
+  <conditionalFormatting sqref="CD6 CD4 CD8 CD10 CD12 CD14 CD16 CD18 CD20 CD22 CD24 CD26 CD28 CD30 CD32 CD34 CD36 CD38 CD40 CD42 CD44 CD46 CD48 CD50 CD52 CD54 CD56 CD58 CD60 CD62 CD64 CD66 CD68 CD70 CD72 CD74 CD76 CD78 CD80 CD82 CD84 CD86 CD88 CD90 CD92 CD94 CD96 CD98 CD100 CD102 CD104">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -69852,7 +69816,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CE6 CE4 CE8 CE10 CE12 CE14 CE16 CE18 CE20 CE22 CE24 CE26 CE28 CE30 CE32 CE34 CE36 CE38 CE40 CE42 CE44 CE46 CE48 CE50 CE52 CE54 CE56 CE58 CE60 CE62 CE64 CE66 CE68 CE70 CE72 CE74 CE76 CE78 CE80 CE82 CE84 CE86 CE88 CE90 CE92 CE94 CE96 CE98 CE100 CE102 CE104">
+  <conditionalFormatting sqref="CE4 CE6 CE8 CE10 CE12 CE14 CE16 CE18 CE20 CE22 CE24 CE26 CE28 CE30 CE32 CE34 CE36 CE38 CE40 CE42 CE44 CE46 CE48 CE50 CE52 CE54 CE56 CE58 CE60 CE62 CE64 CE66 CE68 CE70 CE72 CE74 CE76 CE78 CE80 CE82 CE84 CE86 CE88 CE90 CE92 CE94 CE96 CE98 CE100 CE102 CE104">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -70004,28 +69968,28 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="83"/>
-      <c r="AB2" s="127" t="s">
+      <c r="AB2" s="131" t="s">
         <v>345</v>
       </c>
-      <c r="AC2" s="127"/>
-      <c r="AD2" s="127"/>
-      <c r="AE2" s="127"/>
+      <c r="AC2" s="131"/>
+      <c r="AD2" s="131"/>
+      <c r="AE2" s="131"/>
       <c r="AF2" s="83"/>
       <c r="AG2" s="90"/>
-      <c r="AH2" s="127" t="s">
+      <c r="AH2" s="131" t="s">
         <v>346</v>
       </c>
-      <c r="AI2" s="127"/>
-      <c r="AJ2" s="127"/>
-      <c r="AK2" s="127"/>
+      <c r="AI2" s="131"/>
+      <c r="AJ2" s="131"/>
+      <c r="AK2" s="131"/>
       <c r="AL2" s="83"/>
       <c r="AM2" s="90"/>
-      <c r="AN2" s="127" t="s">
+      <c r="AN2" s="131" t="s">
         <v>347</v>
       </c>
-      <c r="AO2" s="127"/>
-      <c r="AP2" s="127"/>
-      <c r="AQ2" s="127"/>
+      <c r="AO2" s="131"/>
+      <c r="AP2" s="131"/>
+      <c r="AQ2" s="131"/>
       <c r="AR2" s="83"/>
       <c r="AS2" s="83"/>
       <c r="AT2" s="83"/>
@@ -73952,7 +73916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426E89DE-FB26-4184-BD37-CBFF7802F4CC}">
   <dimension ref="A3:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -74052,11 +74016,11 @@
         <v>319</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="144"/>
-      <c r="E8" s="128"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="25"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="128"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="25"/>
       <c r="J8" s="1"/>
       <c r="K8" s="4"/>
@@ -74068,7 +74032,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="144"/>
+      <c r="E9" s="112"/>
       <c r="F9" s="25"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -74088,10 +74052,10 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="144"/>
+      <c r="F10" s="112"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="143"/>
+      <c r="I10" s="111"/>
       <c r="J10" s="6"/>
       <c r="K10" s="1"/>
       <c r="L10" s="5"/>
@@ -74106,8 +74070,8 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="143"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="111"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -74122,11 +74086,11 @@
         <v>320</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="128"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="143"/>
-      <c r="H12" s="144"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="112"/>
       <c r="I12" s="25"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -74138,11 +74102,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="144"/>
-      <c r="F13" s="143"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="111"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="144"/>
+      <c r="I13" s="112"/>
       <c r="J13" s="1" t="s">
         <v>274</v>
       </c>
@@ -74157,8 +74121,8 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="143"/>
-      <c r="F14" s="144"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="112"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -74173,10 +74137,10 @@
       <c r="C15" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D15" s="143"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="144"/>
+      <c r="G15" s="112"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -74192,11 +74156,11 @@
         <v>322</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="128"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="25"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="144"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="112"/>
       <c r="I16" s="25"/>
       <c r="J16" s="1"/>
       <c r="K16" s="4"/>
@@ -74212,7 +74176,7 @@
       <c r="F17" s="25"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="144"/>
+      <c r="I17" s="112"/>
       <c r="J17" s="1" t="s">
         <v>275</v>
       </c>
@@ -74290,7 +74254,7 @@
   <dimension ref="A3:M21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74389,12 +74353,12 @@
         <v>325</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="146"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="146"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
       <c r="J8" s="1"/>
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
@@ -74404,12 +74368,12 @@
       <c r="A9" s="6"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="146"/>
-      <c r="E9" s="146"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="146"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
       <c r="J9" s="8" t="s">
         <v>270</v>
       </c>
@@ -74423,12 +74387,12 @@
         <v>326</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="145"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="6"/>
       <c r="K10" s="1"/>
       <c r="L10" s="5"/>
@@ -74440,16 +74404,16 @@
       <c r="C11" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D11" s="128"/>
-      <c r="E11" s="128"/>
-      <c r="F11" s="128"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M11" s="6"/>
     </row>
@@ -74459,12 +74423,12 @@
         <v>327</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="4"/>
@@ -74474,12 +74438,12 @@
       <c r="A13" s="6"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="146"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
       <c r="J13" s="1" t="s">
         <v>271</v>
       </c>
@@ -74493,12 +74457,12 @@
         <v>328</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="128"/>
-      <c r="F14" s="128"/>
-      <c r="G14" s="128"/>
-      <c r="H14" s="128"/>
-      <c r="I14" s="128"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -74510,12 +74474,12 @@
       <c r="C15" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="128"/>
-      <c r="H15" s="128"/>
-      <c r="I15" s="128"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="5" t="s">
         <v>271</v>
@@ -74529,12 +74493,12 @@
         <v>329</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="146"/>
-      <c r="G16" s="146"/>
-      <c r="H16" s="146"/>
-      <c r="I16" s="146"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
       <c r="J16" s="1"/>
       <c r="K16" s="4"/>
       <c r="L16" s="1"/>
@@ -74544,12 +74508,12 @@
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="146"/>
-      <c r="F17" s="146"/>
-      <c r="G17" s="146"/>
-      <c r="H17" s="146"/>
-      <c r="I17" s="146"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
       <c r="J17" s="1" t="s">
         <v>272</v>
       </c>
@@ -74561,12 +74525,12 @@
       <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
-      <c r="I18" s="128"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="9"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -74576,12 +74540,12 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="128"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>

</xml_diff>